<commit_message>
Update smfGetYahooPortfolioView-Example all elements.xlsx
</commit_message>
<xml_diff>
--- a/docs/samples/smfGetYahooPortfolioView-Example all elements.xlsx
+++ b/docs/samples/smfGetYahooPortfolioView-Example all elements.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SPHD</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>MSFT</t>
+  </si>
+  <si>
+    <t>RY.TO</t>
   </si>
 </sst>
 </file>
@@ -512,7 +515,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,7 +1270,7 @@
         <v>us_market</v>
       </c>
       <c r="I4" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J4" s="11">
         <v>15</v>
@@ -1291,100 +1294,100 @@
         <v>Nasdaq Real Time Price</v>
       </c>
       <c r="Q4" s="10">
-        <v>178.5</v>
+        <v>189.98</v>
       </c>
       <c r="R4" s="1">
-        <v>1686234861</v>
+        <v>1716580800</v>
       </c>
       <c r="S4" s="13">
-        <v>0.67999270000000001</v>
+        <v>3.0999908</v>
       </c>
       <c r="T4" s="1">
-        <v>177.89500000000001</v>
+        <v>188.82</v>
       </c>
       <c r="U4" s="1">
-        <v>178.75</v>
+        <v>190.58</v>
       </c>
       <c r="V4" s="1">
-        <v>177.46</v>
+        <v>188.04040000000001</v>
       </c>
       <c r="W4" s="1">
-        <v>11136909</v>
+        <v>36326975</v>
       </c>
       <c r="X4" s="1">
-        <v>178.03</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="1">
-        <v>178.11</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="1">
-        <v>15728700416</v>
+        <v>15334099968</v>
       </c>
       <c r="AA4" s="1">
-        <v>2807572987904</v>
+        <v>2913172193280</v>
       </c>
       <c r="AB4" s="1">
-        <v>59924909</v>
+        <v>64035801</v>
       </c>
       <c r="AC4" s="1">
-        <v>186.14</v>
+        <v>203.45</v>
       </c>
       <c r="AD4" s="1">
-        <v>385095008000</v>
+        <v>381623009000</v>
       </c>
       <c r="AE4" s="1">
-        <v>7.2905984000000004</v>
+        <v>7.6336389999999996</v>
       </c>
       <c r="AF4" s="1">
-        <v>30.050505000000001</v>
+        <v>29.591899999999999</v>
       </c>
       <c r="AG4" s="1">
-        <v>5.94</v>
+        <v>6.42</v>
       </c>
       <c r="AH4" s="1">
-        <v>1683849600</v>
+        <v>1715299200</v>
       </c>
       <c r="AI4" s="1">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
       <c r="AJ4" s="1">
         <v>5.3E-3</v>
       </c>
       <c r="AK4" s="1">
-        <v>1684368000</v>
+        <v>1715817600</v>
       </c>
       <c r="AL4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="1">
+        <v>5.1369863000000002E-3</v>
+      </c>
+      <c r="AN4" s="1">
         <v>0.96</v>
       </c>
-      <c r="AM4" s="1">
-        <v>5.1737709999999998E-3</v>
-      </c>
-      <c r="AN4" s="1">
-        <v>0.92</v>
-      </c>
       <c r="AO4" s="1">
-        <v>1683234000</v>
+        <v>1714683600</v>
       </c>
       <c r="AP4" s="1">
-        <v>45.15558</v>
+        <v>39.276409999999998</v>
       </c>
       <c r="AQ4" s="1">
-        <v>3.9529999999999998</v>
+        <v>4.8369999999999997</v>
       </c>
       <c r="AR4" s="1">
-        <v>6.56</v>
+        <v>7.23</v>
       </c>
       <c r="AS4" s="1">
-        <v>3.74</v>
+        <v>2.75</v>
       </c>
       <c r="AT4" s="1">
-        <v>27.210364999999999</v>
+        <v>26.276624999999999</v>
       </c>
       <c r="AU4" s="1">
-        <v>123788001280</v>
+        <v>129629003776</v>
       </c>
       <c r="AV4" s="1">
-        <v>2</v>
+        <v>1.66</v>
       </c>
       <c r="AW4" s="1" t="str">
         <v>--</v>
@@ -1393,133 +1396,133 @@
         <v>USD</v>
       </c>
       <c r="AY4" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AZ4" s="1">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BA4" s="1">
-        <v>177.82</v>
+        <v>186.88</v>
       </c>
       <c r="BB4" s="1">
-        <v>3.8240504E-3</v>
+        <v>1.6588135E-2</v>
       </c>
       <c r="BC4" s="1" t="str">
-        <v>177.46 - 178.75</v>
+        <v>188.0404 - 190.58</v>
       </c>
       <c r="BD4" s="1">
-        <v>69115820</v>
+        <v>49758620</v>
       </c>
       <c r="BE4" s="1">
         <v>0</v>
       </c>
       <c r="BF4" s="1">
-        <v>169.53800000000001</v>
+        <v>175.91720000000001</v>
       </c>
       <c r="BG4" s="1">
-        <v>8.9620060000000006</v>
+        <v>14.06279</v>
       </c>
       <c r="BH4" s="1">
-        <v>5.286134E-2</v>
+        <v>7.9939819999999995E-2</v>
       </c>
       <c r="BI4" s="1">
-        <v>152.54669999999999</v>
+        <v>180.9828</v>
       </c>
       <c r="BJ4" s="1">
-        <v>25.953292999999999</v>
+        <v>8.9971920000000001</v>
       </c>
       <c r="BK4" s="1">
-        <v>0.17013341000000001</v>
+        <v>4.9712966999999997E-2</v>
       </c>
       <c r="BL4" s="1" t="str">
-        <v>124.17 - 184.95</v>
+        <v>164.08 - 199.62</v>
       </c>
       <c r="BM4" s="1">
-        <v>124.17</v>
+        <v>164.08</v>
       </c>
       <c r="BN4" s="1">
-        <v>54.33</v>
+        <v>25.899994</v>
       </c>
       <c r="BO4" s="1">
-        <v>0.43754533000000001</v>
+        <v>0.15784978999999999</v>
       </c>
       <c r="BP4" s="1">
-        <v>184.95</v>
+        <v>199.62</v>
       </c>
       <c r="BQ4" s="1">
-        <v>-6.4499969999999998</v>
+        <v>-9.6399989999999995</v>
       </c>
       <c r="BR4" s="1">
-        <v>-3.4874275000000003E-2</v>
-      </c>
-      <c r="BS4" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT4" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU4" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV4" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW4" s="1">
-        <v>1686230999</v>
-      </c>
-      <c r="BX4" s="1">
-        <v>177.89</v>
-      </c>
-      <c r="BY4" s="1">
-        <v>6.9992100000000002E-2</v>
-      </c>
-      <c r="BZ4" s="1">
-        <v>3.93612E-4</v>
+        <v>-4.8291753999999999E-2</v>
+      </c>
+      <c r="BS4" s="1">
+        <v>1716595195</v>
+      </c>
+      <c r="BT4" s="1">
+        <v>189.95</v>
+      </c>
+      <c r="BU4" s="1">
+        <v>-2.9998799999999999E-2</v>
+      </c>
+      <c r="BV4" s="1">
+        <v>-1.5790499999999999E-4</v>
+      </c>
+      <c r="BW4" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX4" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY4" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ4" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA4" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB4" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC4" s="1">
-        <v>0.44052083333333336</v>
+        <v>0.66666666663333329</v>
       </c>
       <c r="CD4" s="1">
-        <v>45058</v>
+        <v>45422</v>
       </c>
       <c r="CE4" s="1">
-        <v>45064</v>
+        <v>45428</v>
       </c>
       <c r="CF4" s="1">
-        <v>45050</v>
-      </c>
-      <c r="CG4" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH4" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI4" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ4" s="1">
-        <v>0.39582175923333335</v>
+        <v>45414</v>
+      </c>
+      <c r="CG4" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH4" s="1">
+        <v>0.83327546293333332</v>
+      </c>
+      <c r="CI4" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ4" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK4" s="1">
-        <v>45085.440520833334</v>
-      </c>
-      <c r="CL4" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM4" s="1">
-        <v>45085.39582175923</v>
+        <v>45436.666666666635</v>
+      </c>
+      <c r="CL4" s="1">
+        <v>45436.833275462937</v>
+      </c>
+      <c r="CM4" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN4" s="1">
-        <v>45133</v>
+        <v>45505</v>
       </c>
       <c r="CO4" s="1">
-        <v>45138</v>
+        <v>45509</v>
       </c>
     </row>
     <row r="5" spans="2:101" x14ac:dyDescent="0.25">
@@ -1545,7 +1548,7 @@
         <v>us_market</v>
       </c>
       <c r="I5" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J5" s="11">
         <v>15</v>
@@ -1569,100 +1572,100 @@
         <v>Nasdaq Real Time Price</v>
       </c>
       <c r="Q5" s="10">
-        <v>324.73</v>
+        <v>430.16</v>
       </c>
       <c r="R5" s="1">
-        <v>1686234861</v>
+        <v>1716580801</v>
       </c>
       <c r="S5" s="13">
-        <v>1.3500061000000001</v>
+        <v>3.1600036999999999</v>
       </c>
       <c r="T5" s="1">
-        <v>323.935</v>
+        <v>427.21</v>
       </c>
       <c r="U5" s="1">
-        <v>325.76990000000001</v>
+        <v>431.05500000000001</v>
       </c>
       <c r="V5" s="1">
-        <v>323.35000000000002</v>
+        <v>424.41</v>
       </c>
       <c r="W5" s="1">
-        <v>6320585</v>
+        <v>11855285</v>
       </c>
       <c r="X5" s="1">
-        <v>325.06</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="1">
-        <v>325.04000000000002</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="1">
-        <v>7435489792</v>
+        <v>7432309760</v>
       </c>
       <c r="AA5" s="1">
-        <v>2414526595072</v>
+        <v>3197082271744</v>
       </c>
       <c r="AB5" s="1">
-        <v>29982609</v>
+        <v>19651666</v>
       </c>
       <c r="AC5" s="1">
-        <v>340.28</v>
+        <v>481.74</v>
       </c>
       <c r="AD5" s="1">
-        <v>207590998000</v>
+        <v>236583993000</v>
       </c>
       <c r="AE5" s="1">
-        <v>11.631171999999999</v>
+        <v>13.513519000000001</v>
       </c>
       <c r="AF5" s="1">
-        <v>35.143940000000001</v>
+        <v>37.30789</v>
       </c>
       <c r="AG5" s="1">
-        <v>9.24</v>
+        <v>11.53</v>
       </c>
       <c r="AH5" s="1">
-        <v>1684281600</v>
+        <v>1715731200</v>
       </c>
       <c r="AI5" s="1">
-        <v>2.6</v>
+        <v>2.86</v>
       </c>
       <c r="AJ5" s="1">
-        <v>8.0999999999999996E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AK5" s="1">
-        <v>1686182400</v>
+        <v>1718236800</v>
       </c>
       <c r="AL5" s="1">
-        <v>2.72</v>
+        <v>3</v>
       </c>
       <c r="AM5" s="1">
-        <v>8.2256169999999993E-3</v>
+        <v>6.861827E-3</v>
       </c>
       <c r="AN5" s="1">
-        <v>2.66</v>
+        <v>2.93</v>
       </c>
       <c r="AO5" s="1">
-        <v>1682458200</v>
+        <v>1714075200</v>
       </c>
       <c r="AP5" s="1">
-        <v>12.404692000000001</v>
+        <v>12.630219</v>
       </c>
       <c r="AQ5" s="1">
-        <v>26.178000000000001</v>
+        <v>34.058</v>
       </c>
       <c r="AR5" s="1">
-        <v>10.95</v>
+        <v>13.26</v>
       </c>
       <c r="AS5" s="1">
-        <v>2.77</v>
+        <v>2.25</v>
       </c>
       <c r="AT5" s="1">
-        <v>29.655709999999999</v>
+        <v>32.440421999999998</v>
       </c>
       <c r="AU5" s="1">
-        <v>100080001024</v>
+        <v>125182001152</v>
       </c>
       <c r="AV5" s="1">
-        <v>1.51</v>
+        <v>2.48</v>
       </c>
       <c r="AW5" s="1" t="str">
         <v>--</v>
@@ -1671,133 +1674,133 @@
         <v>USD</v>
       </c>
       <c r="AY5" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AZ5" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="BA5" s="1">
-        <v>323.38</v>
+        <v>427</v>
       </c>
       <c r="BB5" s="1">
-        <v>4.1746741999999998E-3</v>
+        <v>7.4004769999999999E-3</v>
       </c>
       <c r="BC5" s="1" t="str">
-        <v>323.35 - 325.7699</v>
+        <v>424.41 - 431.055</v>
       </c>
       <c r="BD5" s="1">
-        <v>31379280</v>
+        <v>17052790</v>
       </c>
       <c r="BE5" s="1">
         <v>0</v>
       </c>
       <c r="BF5" s="1">
-        <v>303.84960000000001</v>
+        <v>416.26979999999998</v>
       </c>
       <c r="BG5" s="1">
-        <v>20.880402</v>
+        <v>13.890198</v>
       </c>
       <c r="BH5" s="1">
-        <v>6.8719530000000001E-2</v>
+        <v>3.3368255999999999E-2</v>
       </c>
       <c r="BI5" s="1">
-        <v>261.83465999999999</v>
+        <v>376.96724999999998</v>
       </c>
       <c r="BJ5" s="1">
-        <v>62.895355000000002</v>
+        <v>53.192749999999997</v>
       </c>
       <c r="BK5" s="1">
-        <v>0.24021020000000001</v>
+        <v>0.14110708</v>
       </c>
       <c r="BL5" s="1" t="str">
-        <v>213.43 - 338.56</v>
+        <v>309.45 - 433.6</v>
       </c>
       <c r="BM5" s="1">
-        <v>213.43</v>
+        <v>309.45</v>
       </c>
       <c r="BN5" s="1">
-        <v>111.30002</v>
+        <v>120.70999</v>
       </c>
       <c r="BO5" s="1">
-        <v>0.52148249999999996</v>
+        <v>0.39007913999999999</v>
       </c>
       <c r="BP5" s="1">
-        <v>338.56</v>
+        <v>433.6</v>
       </c>
       <c r="BQ5" s="1">
-        <v>-13.829986999999999</v>
+        <v>-3.4400024</v>
       </c>
       <c r="BR5" s="1">
-        <v>-4.0849440000000001E-2</v>
-      </c>
-      <c r="BS5" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT5" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU5" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV5" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW5" s="1">
-        <v>1686230999</v>
-      </c>
-      <c r="BX5" s="1">
-        <v>324</v>
-      </c>
-      <c r="BY5" s="1">
-        <v>0.61999499999999996</v>
-      </c>
-      <c r="BZ5" s="1">
-        <v>1.91723E-3</v>
+        <v>-7.9335849999999999E-3</v>
+      </c>
+      <c r="BS5" s="1">
+        <v>1716595174</v>
+      </c>
+      <c r="BT5" s="1">
+        <v>430.32499999999999</v>
+      </c>
+      <c r="BU5" s="1">
+        <v>0.16500899999999999</v>
+      </c>
+      <c r="BV5" s="1">
+        <v>3.8359800000000002E-4</v>
+      </c>
+      <c r="BW5" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX5" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY5" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ5" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA5" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB5" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC5" s="1">
-        <v>0.44052083333333336</v>
+        <v>0.66667824073333326</v>
       </c>
       <c r="CD5" s="1">
-        <v>45063</v>
+        <v>45427</v>
       </c>
       <c r="CE5" s="1">
-        <v>45085</v>
+        <v>45456</v>
       </c>
       <c r="CF5" s="1">
-        <v>45041</v>
-      </c>
-      <c r="CG5" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH5" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI5" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ5" s="1">
-        <v>0.39582175923333335</v>
+        <v>45407</v>
+      </c>
+      <c r="CG5" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH5" s="1">
+        <v>0.83303240743333329</v>
+      </c>
+      <c r="CI5" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ5" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK5" s="1">
-        <v>45085.440520833334</v>
-      </c>
-      <c r="CL5" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM5" s="1">
-        <v>45085.39582175923</v>
+        <v>45436.666678240734</v>
+      </c>
+      <c r="CL5" s="1">
+        <v>45436.833032407434</v>
+      </c>
+      <c r="CM5" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN5" s="1">
-        <v>45131</v>
+        <v>45496</v>
       </c>
       <c r="CO5" s="1">
-        <v>45135</v>
+        <v>45502</v>
       </c>
     </row>
     <row r="6" spans="2:101" x14ac:dyDescent="0.25">
@@ -1823,7 +1826,7 @@
         <v>us_market</v>
       </c>
       <c r="I6" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J6" s="11">
         <v>15</v>
@@ -1844,103 +1847,103 @@
         <v>EQUITY</v>
       </c>
       <c r="P6" s="12" t="str">
-        <v>Nasdaq Real Time Price</v>
+        <v>Delayed Quote</v>
       </c>
       <c r="Q6" s="10">
-        <v>93.435000000000002</v>
+        <v>94.43</v>
       </c>
       <c r="R6" s="1">
-        <v>1686234840</v>
+        <v>1716580802</v>
       </c>
       <c r="S6" s="13">
-        <v>-0.10500336</v>
+        <v>0.559998</v>
       </c>
       <c r="T6" s="1">
-        <v>92.38</v>
+        <v>94.1</v>
       </c>
       <c r="U6" s="1">
-        <v>93.66</v>
+        <v>94.6</v>
       </c>
       <c r="V6" s="1">
-        <v>92.32</v>
+        <v>93.74</v>
       </c>
       <c r="W6" s="1">
-        <v>217350</v>
+        <v>1639105</v>
       </c>
       <c r="X6" s="1">
-        <v>93.56</v>
+        <v>94.03</v>
       </c>
       <c r="Y6" s="1">
-        <v>93.56</v>
+        <v>94.86</v>
       </c>
       <c r="Z6" s="1">
-        <v>346540000</v>
+        <v>345835008</v>
       </c>
       <c r="AA6" s="1">
-        <v>32378963968</v>
+        <v>32657199104</v>
       </c>
       <c r="AB6" s="1">
-        <v>1946633</v>
+        <v>1925461</v>
       </c>
       <c r="AC6" s="1">
-        <v>90.25</v>
+        <v>90.82</v>
       </c>
       <c r="AD6" s="1">
-        <v>16012999700</v>
+        <v>14540000300</v>
       </c>
       <c r="AE6" s="1">
-        <v>2.0220422999999998</v>
+        <v>2.2460246000000001</v>
       </c>
       <c r="AF6" s="1">
-        <v>13.328815000000001</v>
+        <v>18.020992</v>
       </c>
       <c r="AG6" s="1">
-        <v>7.01</v>
+        <v>5.24</v>
       </c>
       <c r="AH6" s="1">
-        <v>1684195200</v>
+        <v>1715644800</v>
       </c>
       <c r="AI6" s="1">
-        <v>3.18</v>
+        <v>3.26</v>
       </c>
       <c r="AJ6" s="1">
-        <v>3.5099999999999999E-2</v>
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="AK6" s="1">
-        <v>1686787200</v>
+        <v>1718323200</v>
       </c>
       <c r="AL6" s="1">
-        <v>3.24</v>
+        <v>3.32</v>
       </c>
       <c r="AM6" s="1">
-        <v>3.3996150000000003E-2</v>
+        <v>3.4728879999999997E-2</v>
       </c>
       <c r="AN6" s="1">
-        <v>3.18</v>
+        <v>3.26</v>
       </c>
       <c r="AO6" s="1">
-        <v>1683235758</v>
+        <v>1714680000</v>
       </c>
       <c r="AP6" s="1">
-        <v>1.5510458</v>
+        <v>1.5115814000000001</v>
       </c>
       <c r="AQ6" s="1">
-        <v>60.24</v>
+        <v>62.470999999999997</v>
       </c>
       <c r="AR6" s="1">
-        <v>5.23</v>
+        <v>5.61</v>
       </c>
       <c r="AS6" s="1">
-        <v>3.15</v>
+        <v>2.89</v>
       </c>
       <c r="AT6" s="1">
-        <v>17.865200000000002</v>
+        <v>16.832440999999999</v>
       </c>
       <c r="AU6" s="1">
-        <v>5190000128</v>
+        <v>5257999872</v>
       </c>
       <c r="AV6" s="1">
-        <v>4.96</v>
+        <v>3.4</v>
       </c>
       <c r="AW6" s="1" t="str">
         <v>--</v>
@@ -1949,133 +1952,133 @@
         <v>USD</v>
       </c>
       <c r="AY6" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AZ6" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="BA6" s="1">
-        <v>93.54</v>
+        <v>93.87</v>
       </c>
       <c r="BB6" s="1">
-        <v>-1.1225503E-3</v>
+        <v>5.9656700000000002E-3</v>
       </c>
       <c r="BC6" s="1" t="str">
-        <v>92.32 - 93.66</v>
+        <v>93.74 - 94.6</v>
       </c>
       <c r="BD6" s="1">
-        <v>2321990</v>
+        <v>1908320</v>
       </c>
       <c r="BE6" s="1">
         <v>0</v>
       </c>
       <c r="BF6" s="1">
-        <v>96.712400000000002</v>
+        <v>92.569199999999995</v>
       </c>
       <c r="BG6" s="1">
-        <v>-3.2774047999999998</v>
+        <v>1.8608016999999999</v>
       </c>
       <c r="BH6" s="1">
-        <v>-3.3888153999999997E-2</v>
+        <v>2.0101737000000001E-2</v>
       </c>
       <c r="BI6" s="1">
-        <v>94.051950000000005</v>
+        <v>90.263549999999995</v>
       </c>
       <c r="BJ6" s="1">
-        <v>-0.61695100000000003</v>
+        <v>4.1664504999999998</v>
       </c>
       <c r="BK6" s="1">
-        <v>-6.5596830000000002E-3</v>
+        <v>4.6158726999999997E-2</v>
       </c>
       <c r="BL6" s="1" t="str">
-        <v>78.1 - 102.21</v>
+        <v>80.46 - 98.85</v>
       </c>
       <c r="BM6" s="1">
-        <v>78.099999999999994</v>
+        <v>80.459999999999994</v>
       </c>
       <c r="BN6" s="1">
-        <v>15.334999</v>
+        <v>13.970001</v>
       </c>
       <c r="BO6" s="1">
-        <v>0.19635083</v>
+        <v>0.17362665999999999</v>
       </c>
       <c r="BP6" s="1">
-        <v>102.21</v>
+        <v>98.85</v>
       </c>
       <c r="BQ6" s="1">
-        <v>-8.7750020000000006</v>
+        <v>-4.4199979999999996</v>
       </c>
       <c r="BR6" s="1">
-        <v>-8.5852675000000003E-2</v>
-      </c>
-      <c r="BS6" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT6" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU6" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV6" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW6" s="1">
-        <v>1686230860</v>
-      </c>
-      <c r="BX6" s="1">
-        <v>92.72</v>
-      </c>
-      <c r="BY6" s="1">
-        <v>-0.82</v>
-      </c>
-      <c r="BZ6" s="1">
-        <v>-8.7662999999999994E-3</v>
+        <v>-4.4714193999999999E-2</v>
+      </c>
+      <c r="BS6" s="1">
+        <v>1716585866</v>
+      </c>
+      <c r="BT6" s="1">
+        <v>94.43</v>
+      </c>
+      <c r="BU6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BV6" s="1">
+        <v>0</v>
+      </c>
+      <c r="BW6" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX6" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY6" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ6" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA6" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB6" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC6" s="1">
-        <v>0.44027777773333332</v>
+        <v>0.66668981483333334</v>
       </c>
       <c r="CD6" s="1">
-        <v>45062</v>
+        <v>45426</v>
       </c>
       <c r="CE6" s="1">
-        <v>45092</v>
+        <v>45457</v>
       </c>
       <c r="CF6" s="1">
-        <v>45050</v>
-      </c>
-      <c r="CG6" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH6" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI6" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ6" s="1">
-        <v>0.3942129629333333</v>
+        <v>45414</v>
+      </c>
+      <c r="CG6" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH6" s="1">
+        <v>0.7253009259333334</v>
+      </c>
+      <c r="CI6" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ6" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK6" s="1">
-        <v>45085.440277777729</v>
-      </c>
-      <c r="CL6" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM6" s="1">
-        <v>45085.394212962929</v>
+        <v>45436.66668981484</v>
+      </c>
+      <c r="CL6" s="1">
+        <v>45436.725300925937</v>
+      </c>
+      <c r="CM6" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN6" s="1">
-        <v>45140</v>
+        <v>45505</v>
       </c>
       <c r="CO6" s="1">
-        <v>45145</v>
+        <v>45509</v>
       </c>
     </row>
     <row r="7" spans="2:101" x14ac:dyDescent="0.25">
@@ -2101,7 +2104,7 @@
         <v>us_market</v>
       </c>
       <c r="I7" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J7" s="11">
         <v>15</v>
@@ -2122,103 +2125,103 @@
         <v>EQUITY</v>
       </c>
       <c r="P7" s="12" t="str">
-        <v>Nasdaq Real Time Price</v>
+        <v>Delayed Quote</v>
       </c>
       <c r="Q7" s="10">
-        <v>284.83</v>
+        <v>258.11</v>
       </c>
       <c r="R7" s="1">
-        <v>1686234850</v>
+        <v>1716580802</v>
       </c>
       <c r="S7" s="13">
-        <v>2.9299927000000001</v>
+        <v>0.17999299999999999</v>
       </c>
       <c r="T7" s="1">
-        <v>280.97000000000003</v>
+        <v>258.74</v>
       </c>
       <c r="U7" s="1">
-        <v>284.88</v>
+        <v>260.45999999999998</v>
       </c>
       <c r="V7" s="1">
-        <v>280</v>
+        <v>257.52</v>
       </c>
       <c r="W7" s="1">
-        <v>1011712</v>
+        <v>3382879</v>
       </c>
       <c r="X7" s="1">
-        <v>284.27999999999997</v>
+        <v>257.7</v>
       </c>
       <c r="Y7" s="1">
-        <v>284.3</v>
+        <v>258.39999999999998</v>
       </c>
       <c r="Z7" s="1">
-        <v>730094016</v>
+        <v>720681984</v>
       </c>
       <c r="AA7" s="1">
-        <v>207952674816</v>
+        <v>186015219712</v>
       </c>
       <c r="AB7" s="1">
-        <v>2600280</v>
+        <v>3372761</v>
       </c>
       <c r="AC7" s="1">
-        <v>318.77999999999997</v>
+        <v>314.22000000000003</v>
       </c>
       <c r="AD7" s="1">
-        <v>23414800400</v>
+        <v>25764700200</v>
       </c>
       <c r="AE7" s="1">
-        <v>8.8812490000000004</v>
+        <v>7.2197703999999998</v>
       </c>
       <c r="AF7" s="1">
-        <v>30.626878999999999</v>
+        <v>21.929480000000002</v>
       </c>
       <c r="AG7" s="1">
-        <v>9.3000000000000007</v>
+        <v>11.77</v>
       </c>
       <c r="AH7" s="1">
-        <v>1685664000</v>
+        <v>1717372800</v>
       </c>
       <c r="AI7" s="1">
-        <v>5.8</v>
+        <v>6.38</v>
       </c>
       <c r="AJ7" s="1">
-        <v>2.1399999999999999E-2</v>
+        <v>2.5899999999999999E-2</v>
       </c>
       <c r="AK7" s="1">
-        <v>1687219200</v>
+        <v>1718582400</v>
       </c>
       <c r="AL7" s="1">
-        <v>6.08</v>
+        <v>6.68</v>
       </c>
       <c r="AM7" s="1">
-        <v>2.0574671999999999E-2</v>
+        <v>2.4735395E-2</v>
       </c>
       <c r="AN7" s="1">
-        <v>5.8</v>
+        <v>6.38</v>
       </c>
       <c r="AO7" s="1">
-        <v>1682425800</v>
+        <v>1714480200</v>
       </c>
       <c r="AP7" s="1">
-        <v>-36.004294999999999</v>
+        <v>-38.489409999999999</v>
       </c>
       <c r="AQ7" s="1">
-        <v>-7.9109999999999996</v>
+        <v>-6.7060000000000004</v>
       </c>
       <c r="AR7" s="1">
-        <v>12.11</v>
+        <v>13.28</v>
       </c>
       <c r="AS7" s="1">
-        <v>3.07</v>
+        <v>3.17</v>
       </c>
       <c r="AT7" s="1">
-        <v>23.520230999999999</v>
+        <v>19.435993</v>
       </c>
       <c r="AU7" s="1">
-        <v>12514100224</v>
+        <v>13809500160</v>
       </c>
       <c r="AV7" s="1">
-        <v>2.85</v>
+        <v>2.21</v>
       </c>
       <c r="AW7" s="1" t="str">
         <v>--</v>
@@ -2227,133 +2230,133 @@
         <v>USD</v>
       </c>
       <c r="AY7" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AZ7" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="BA7" s="1">
-        <v>281.89999999999998</v>
+        <v>257.93</v>
       </c>
       <c r="BB7" s="1">
-        <v>1.039373E-2</v>
+        <v>6.9783499999999995E-4</v>
       </c>
       <c r="BC7" s="1" t="str">
-        <v>280.0 - 284.88</v>
+        <v>257.52 - 260.46</v>
       </c>
       <c r="BD7" s="1">
-        <v>2748320</v>
+        <v>3069790</v>
       </c>
       <c r="BE7" s="1">
         <v>0</v>
       </c>
       <c r="BF7" s="1">
-        <v>289.27179999999998</v>
+        <v>272.74</v>
       </c>
       <c r="BG7" s="1">
-        <v>-4.4418030000000002</v>
+        <v>-14.630005000000001</v>
       </c>
       <c r="BH7" s="1">
-        <v>-1.53551195E-2</v>
+        <v>-5.3640849999999997E-2</v>
       </c>
       <c r="BI7" s="1">
-        <v>269.55606</v>
+        <v>278.80489999999998</v>
       </c>
       <c r="BJ7" s="1">
-        <v>15.273925999999999</v>
+        <v>-20.694915999999999</v>
       </c>
       <c r="BK7" s="1">
-        <v>5.6663263999999998E-2</v>
+        <v>-7.4227230000000005E-2</v>
       </c>
       <c r="BL7" s="1" t="str">
-        <v>230.58 - 298.86</v>
+        <v>245.73 - 302.39</v>
       </c>
       <c r="BM7" s="1">
-        <v>230.58</v>
+        <v>245.73</v>
       </c>
       <c r="BN7" s="1">
-        <v>54.249985000000002</v>
+        <v>12.379989999999999</v>
       </c>
       <c r="BO7" s="1">
-        <v>0.23527619</v>
+        <v>5.0380456999999997E-2</v>
       </c>
       <c r="BP7" s="1">
-        <v>298.86</v>
+        <v>302.39</v>
       </c>
       <c r="BQ7" s="1">
-        <v>-14.029999</v>
+        <v>-44.280029999999996</v>
       </c>
       <c r="BR7" s="1">
-        <v>-4.6945057999999998E-2</v>
-      </c>
-      <c r="BS7" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT7" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU7" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV7" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW7" s="1">
-        <v>1686230987</v>
-      </c>
-      <c r="BX7" s="1">
-        <v>281.75</v>
-      </c>
-      <c r="BY7" s="1">
-        <v>-0.14999399999999999</v>
-      </c>
-      <c r="BZ7" s="1">
-        <v>-5.3208200000000002E-4</v>
+        <v>-0.14643349999999999</v>
+      </c>
+      <c r="BS7" s="1">
+        <v>1716595170</v>
+      </c>
+      <c r="BT7" s="1">
+        <v>258.39</v>
+      </c>
+      <c r="BU7" s="1">
+        <v>0.28002929999999998</v>
+      </c>
+      <c r="BV7" s="1">
+        <v>1.0849224E-3</v>
+      </c>
+      <c r="BW7" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX7" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY7" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ7" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA7" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB7" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC7" s="1">
-        <v>0.44039351853333331</v>
+        <v>0.66668981483333334</v>
       </c>
       <c r="CD7" s="1">
-        <v>45079</v>
+        <v>45446</v>
       </c>
       <c r="CE7" s="1">
-        <v>45097</v>
+        <v>45460</v>
       </c>
       <c r="CF7" s="1">
-        <v>45041</v>
-      </c>
-      <c r="CG7" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH7" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI7" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ7" s="1">
-        <v>0.39568287033333338</v>
+        <v>45412</v>
+      </c>
+      <c r="CG7" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH7" s="1">
+        <v>0.83298611113333332</v>
+      </c>
+      <c r="CI7" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ7" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK7" s="1">
-        <v>45085.440393518533</v>
-      </c>
-      <c r="CL7" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM7" s="1">
-        <v>45085.395682870338</v>
+        <v>45436.66668981484</v>
+      </c>
+      <c r="CL7" s="1">
+        <v>45436.832986111134</v>
+      </c>
+      <c r="CM7" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN7" s="1">
-        <v>45131</v>
+        <v>45498</v>
       </c>
       <c r="CO7" s="1">
-        <v>45135</v>
+        <v>45502</v>
       </c>
     </row>
     <row r="8" spans="2:101" x14ac:dyDescent="0.25">
@@ -2379,7 +2382,7 @@
         <v>us_market</v>
       </c>
       <c r="I8" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J8" s="11">
         <v>15</v>
@@ -2403,100 +2406,100 @@
         <v>Nasdaq Real Time Price</v>
       </c>
       <c r="Q8" s="10">
-        <v>44.06</v>
+        <v>36.229999999999997</v>
       </c>
       <c r="R8" s="1">
-        <v>1686234605</v>
+        <v>1716580802</v>
       </c>
       <c r="S8" s="13">
-        <v>-0.25</v>
+        <v>-0.5</v>
       </c>
       <c r="T8" s="1">
-        <v>44.29</v>
+        <v>36.130000000000003</v>
       </c>
       <c r="U8" s="1">
-        <v>44.35</v>
+        <v>36.6</v>
       </c>
       <c r="V8" s="1">
-        <v>43.84</v>
+        <v>36.090000000000003</v>
       </c>
       <c r="W8" s="1">
-        <v>23460</v>
+        <v>245734</v>
       </c>
       <c r="X8" s="1">
-        <v>44.03</v>
+        <v>36.01</v>
       </c>
       <c r="Y8" s="1">
-        <v>44.14</v>
+        <v>36.57</v>
       </c>
       <c r="Z8" s="1">
-        <v>35965600</v>
+        <v>38028100</v>
       </c>
       <c r="AA8" s="1">
-        <v>1584644352</v>
+        <v>1377758080</v>
       </c>
       <c r="AB8" s="1">
-        <v>158428</v>
+        <v>272596</v>
       </c>
       <c r="AC8" s="1">
-        <v>53</v>
+        <v>43.5</v>
       </c>
       <c r="AD8" s="1">
-        <v>1149474940</v>
+        <v>1168521980</v>
       </c>
       <c r="AE8" s="1">
-        <v>1.3785810000000001</v>
+        <v>1.1790605000000001</v>
       </c>
       <c r="AF8" s="1">
-        <v>16.021818</v>
+        <v>15.960352</v>
       </c>
       <c r="AG8" s="1">
-        <v>2.75</v>
+        <v>2.27</v>
       </c>
       <c r="AH8" s="1">
-        <v>1682553600</v>
+        <v>1714348800</v>
       </c>
       <c r="AI8" s="1">
-        <v>1.94</v>
+        <v>1.95</v>
       </c>
       <c r="AJ8" s="1">
-        <v>4.3799999999999999E-2</v>
+        <v>5.3800000000000001E-2</v>
       </c>
       <c r="AK8" s="1">
-        <v>1684108800</v>
+        <v>1715731200</v>
       </c>
       <c r="AL8" s="1">
-        <v>1.94</v>
+        <v>1.95</v>
       </c>
       <c r="AM8" s="1">
-        <v>4.3669595999999998E-2</v>
+        <v>5.2953991999999998E-2</v>
       </c>
       <c r="AN8" s="1">
-        <v>1.9350000000000001</v>
+        <v>1.9450000000000001</v>
       </c>
       <c r="AO8" s="1">
-        <v>1683212400</v>
+        <v>1714989600</v>
       </c>
       <c r="AP8" s="1">
-        <v>1.2681327</v>
+        <v>1.0255612000000001</v>
       </c>
       <c r="AQ8" s="1">
-        <v>34.744</v>
+        <v>35.326999999999998</v>
       </c>
       <c r="AR8" s="1">
-        <v>2.79</v>
+        <v>2.81</v>
       </c>
       <c r="AS8" s="1">
-        <v>5.79</v>
+        <v>5.75</v>
       </c>
       <c r="AT8" s="1">
-        <v>15.792115000000001</v>
+        <v>12.893238</v>
       </c>
       <c r="AU8" s="1">
-        <v>330449984</v>
+        <v>325575008</v>
       </c>
       <c r="AV8" s="1">
-        <v>3.18</v>
+        <v>4.01</v>
       </c>
       <c r="AW8" s="1" t="str">
         <v>--</v>
@@ -2505,76 +2508,76 @@
         <v>USD</v>
       </c>
       <c r="AY8" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AZ8" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BA8" s="1">
-        <v>44.31</v>
+        <v>36.729999999999997</v>
       </c>
       <c r="BB8" s="1">
-        <v>-5.6420669999999997E-3</v>
+        <v>-1.3612900000000001E-2</v>
       </c>
       <c r="BC8" s="1" t="str">
-        <v>43.84 - 44.35</v>
+        <v>36.09 - 36.6</v>
       </c>
       <c r="BD8" s="1">
-        <v>171790</v>
+        <v>215300</v>
       </c>
       <c r="BE8" s="1">
         <v>0</v>
       </c>
       <c r="BF8" s="1">
-        <v>46.119199999999999</v>
+        <v>37.308799999999998</v>
       </c>
       <c r="BG8" s="1">
-        <v>-2.0592003000000001</v>
+        <v>-1.0788002000000001</v>
       </c>
       <c r="BH8" s="1">
-        <v>-4.4649523000000003E-2</v>
+        <v>-2.8915435E-2</v>
       </c>
       <c r="BI8" s="1">
-        <v>47.303699999999999</v>
+        <v>38.0535</v>
       </c>
       <c r="BJ8" s="1">
-        <v>-3.2436981</v>
+        <v>-1.8235015999999999</v>
       </c>
       <c r="BK8" s="1">
-        <v>-6.8571759999999995E-2</v>
+        <v>-4.7919419999999997E-2</v>
       </c>
       <c r="BL8" s="1" t="str">
-        <v>41.83 - 54.89</v>
+        <v>34.95 - 44.9</v>
       </c>
       <c r="BM8" s="1">
-        <v>41.83</v>
+        <v>34.950000000000003</v>
       </c>
       <c r="BN8" s="1">
-        <v>2.2299994999999999</v>
+        <v>1.2799988</v>
       </c>
       <c r="BO8" s="1">
-        <v>5.3311009999999999E-2</v>
+        <v>3.6623713000000002E-2</v>
       </c>
       <c r="BP8" s="1">
-        <v>54.89</v>
+        <v>44.9</v>
       </c>
       <c r="BQ8" s="1">
-        <v>-10.829998</v>
+        <v>-8.6700020000000002</v>
       </c>
       <c r="BR8" s="1">
-        <v>-0.19730366999999999</v>
-      </c>
-      <c r="BS8" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT8" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU8" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV8" s="1" t="str">
-        <v>--</v>
+        <v>-0.19309580000000001</v>
+      </c>
+      <c r="BS8" s="1">
+        <v>1716591102</v>
+      </c>
+      <c r="BT8" s="1">
+        <v>36.28</v>
+      </c>
+      <c r="BU8" s="1">
+        <v>4.9999200000000001E-2</v>
+      </c>
+      <c r="BV8" s="1">
+        <v>1.3800500000000001E-3</v>
       </c>
       <c r="BW8" s="1" t="str">
         <v>--</v>
@@ -2592,25 +2595,25 @@
         <v>false</v>
       </c>
       <c r="CB8" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC8" s="1">
-        <v>0.43755787033333332</v>
+        <v>0.66668981483333334</v>
       </c>
       <c r="CD8" s="1">
-        <v>45043</v>
+        <v>45411</v>
       </c>
       <c r="CE8" s="1">
-        <v>45061</v>
+        <v>45427</v>
       </c>
       <c r="CF8" s="1">
-        <v>45050</v>
-      </c>
-      <c r="CG8" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH8" s="1" t="str">
-        <v>--</v>
+        <v>45418</v>
+      </c>
+      <c r="CG8" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH8" s="1">
+        <v>0.78590277773333328</v>
       </c>
       <c r="CI8" s="1" t="str">
         <v>--</v>
@@ -2619,19 +2622,19 @@
         <v>--</v>
       </c>
       <c r="CK8" s="1">
-        <v>45085.437557870333</v>
-      </c>
-      <c r="CL8" s="1" t="str">
-        <v>--</v>
+        <v>45436.66668981484</v>
+      </c>
+      <c r="CL8" s="1">
+        <v>45436.78590277773</v>
       </c>
       <c r="CM8" s="1" t="str">
         <v>--</v>
       </c>
       <c r="CN8" s="1">
-        <v>45140</v>
+        <v>45505</v>
       </c>
       <c r="CO8" s="1">
-        <v>45145</v>
+        <v>45509</v>
       </c>
     </row>
     <row r="9" spans="2:101" x14ac:dyDescent="0.25">
@@ -2933,7 +2936,7 @@
         <v>us_market</v>
       </c>
       <c r="I10" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J10" s="11">
         <v>15</v>
@@ -2957,31 +2960,31 @@
         <v>Nasdaq Real Time Price</v>
       </c>
       <c r="Q10" s="10">
-        <v>40.869999999999997</v>
+        <v>44.31</v>
       </c>
       <c r="R10" s="1">
-        <v>1686234857</v>
+        <v>1716580800</v>
       </c>
       <c r="S10" s="13">
-        <v>-0.27000046</v>
+        <v>9.0000200000000002E-2</v>
       </c>
       <c r="T10" s="1">
-        <v>41.1</v>
+        <v>44.44</v>
       </c>
       <c r="U10" s="1">
-        <v>41.12</v>
+        <v>44.5</v>
       </c>
       <c r="V10" s="1">
-        <v>40.76</v>
+        <v>44.234999999999999</v>
       </c>
       <c r="W10" s="1">
-        <v>317297</v>
+        <v>387173</v>
       </c>
       <c r="X10" s="1">
-        <v>40.880000000000003</v>
+        <v>44.2</v>
       </c>
       <c r="Y10" s="1">
-        <v>40.89</v>
+        <v>45.56</v>
       </c>
       <c r="Z10" s="1" t="str">
         <v>--</v>
@@ -2990,7 +2993,7 @@
         <v>--</v>
       </c>
       <c r="AB10" s="1">
-        <v>785422</v>
+        <v>589520</v>
       </c>
       <c r="AC10" s="1" t="str">
         <v>--</v>
@@ -3002,7 +3005,7 @@
         <v>--</v>
       </c>
       <c r="AF10" s="1">
-        <v>16.096802</v>
+        <v>17.45166</v>
       </c>
       <c r="AG10" s="1">
         <v>2.5390136000000001</v>
@@ -3014,7 +3017,7 @@
         <v>--</v>
       </c>
       <c r="AJ10" s="1">
-        <v>4.3999999999999997E-2</v>
+        <v>4.36E-2</v>
       </c>
       <c r="AK10" s="1" t="str">
         <v>--</v>
@@ -3059,97 +3062,97 @@
         <v>USD</v>
       </c>
       <c r="AY10" s="1">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="AZ10" s="1">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="BA10" s="1">
-        <v>41.14</v>
+        <v>44.22</v>
       </c>
       <c r="BB10" s="1">
-        <v>-6.5629670000000003E-3</v>
+        <v>2.03528E-3</v>
       </c>
       <c r="BC10" s="1" t="str">
-        <v>40.76 - 41.12</v>
+        <v>44.235 - 44.5</v>
       </c>
       <c r="BD10" s="1">
-        <v>980190</v>
+        <v>444810</v>
       </c>
       <c r="BE10" s="1">
         <v>0</v>
       </c>
       <c r="BF10" s="1">
-        <v>41.198599999999999</v>
+        <v>43.872599999999998</v>
       </c>
       <c r="BG10" s="1">
-        <v>-0.32860183999999998</v>
+        <v>0.43740082000000002</v>
       </c>
       <c r="BH10" s="1">
-        <v>-7.9760439999999998E-3</v>
+        <v>9.9697940000000006E-3</v>
       </c>
       <c r="BI10" s="1">
-        <v>42.775350000000003</v>
+        <v>41.617899999999999</v>
       </c>
       <c r="BJ10" s="1">
-        <v>-1.9053496999999999</v>
+        <v>2.6921005</v>
       </c>
       <c r="BK10" s="1">
-        <v>-4.4543172999999998E-2</v>
+        <v>6.468612E-2</v>
       </c>
       <c r="BL10" s="1" t="str">
-        <v>38.33 - 47.31</v>
+        <v>37.19 - 45.44</v>
       </c>
       <c r="BM10" s="1">
-        <v>38.33</v>
+        <v>37.19</v>
       </c>
       <c r="BN10" s="1">
-        <v>2.5399970000000001</v>
+        <v>7.1200026999999997</v>
       </c>
       <c r="BO10" s="1">
-        <v>6.6266549999999994E-2</v>
+        <v>0.19144939</v>
       </c>
       <c r="BP10" s="1">
-        <v>47.31</v>
+        <v>45.44</v>
       </c>
       <c r="BQ10" s="1">
-        <v>-6.4400024</v>
+        <v>-1.1299973000000001</v>
       </c>
       <c r="BR10" s="1">
-        <v>-0.13612350000000001</v>
-      </c>
-      <c r="BS10" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT10" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU10" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV10" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW10" s="1">
-        <v>1686230997</v>
-      </c>
-      <c r="BX10" s="1">
-        <v>41.14</v>
-      </c>
-      <c r="BY10" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ10" s="1">
-        <v>0</v>
+        <v>-2.4867897999999999E-2</v>
+      </c>
+      <c r="BS10" s="1">
+        <v>1716593968</v>
+      </c>
+      <c r="BT10" s="1">
+        <v>44.2</v>
+      </c>
+      <c r="BU10" s="1">
+        <v>-0.110001</v>
+      </c>
+      <c r="BV10" s="1">
+        <v>-2.4825200000000002E-3</v>
+      </c>
+      <c r="BW10" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX10" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY10" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ10" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA10" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB10" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC10" s="1">
-        <v>0.44047453703333334</v>
+        <v>0.66666666663333329</v>
       </c>
       <c r="CD10" s="1" t="str">
         <v>--</v>
@@ -3160,26 +3163,26 @@
       <c r="CF10" s="1" t="str">
         <v>--</v>
       </c>
-      <c r="CG10" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH10" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI10" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ10" s="1">
-        <v>0.39579861113333337</v>
+      <c r="CG10" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH10" s="1">
+        <v>0.81907407403333332</v>
+      </c>
+      <c r="CI10" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ10" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK10" s="1">
-        <v>45085.440474537034</v>
-      </c>
-      <c r="CL10" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM10" s="1">
-        <v>45085.395798611135</v>
+        <v>45436.666666666635</v>
+      </c>
+      <c r="CL10" s="1">
+        <v>45436.819074074039</v>
+      </c>
+      <c r="CM10" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN10" s="1" t="str">
         <v>--</v>
@@ -3487,7 +3490,7 @@
         <v>us_market</v>
       </c>
       <c r="I12" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J12" s="11">
         <v>15</v>
@@ -3508,103 +3511,103 @@
         <v>EQUITY</v>
       </c>
       <c r="P12" s="12" t="str">
-        <v>Nasdaq Real Time Price</v>
+        <v>Delayed Quote</v>
       </c>
       <c r="Q12" s="10">
-        <v>108.5401</v>
+        <v>113.42</v>
       </c>
       <c r="R12" s="1">
-        <v>1686234861</v>
+        <v>1716580944</v>
       </c>
       <c r="S12" s="13">
-        <v>1.0101318E-2</v>
+        <v>-9.0004000000000001E-2</v>
       </c>
       <c r="T12" s="1">
-        <v>108.77</v>
+        <v>114.84</v>
       </c>
       <c r="U12" s="1">
-        <v>109.14</v>
+        <v>115.08</v>
       </c>
       <c r="V12" s="1">
-        <v>108.1</v>
+        <v>113.035</v>
       </c>
       <c r="W12" s="1">
-        <v>2016857</v>
+        <v>12212949</v>
       </c>
       <c r="X12" s="1">
-        <v>108.68</v>
+        <v>113.42</v>
       </c>
       <c r="Y12" s="1">
-        <v>108.67</v>
+        <v>113.59</v>
       </c>
       <c r="Z12" s="1">
-        <v>4042980096</v>
+        <v>4485929984</v>
       </c>
       <c r="AA12" s="1">
-        <v>438825451520</v>
+        <v>508794175488</v>
       </c>
       <c r="AB12" s="1">
-        <v>16329811</v>
+        <v>18006182</v>
       </c>
       <c r="AC12" s="1">
-        <v>127.56</v>
+        <v>132.88</v>
       </c>
       <c r="AD12" s="1">
-        <v>398438007000</v>
+        <v>335350989000</v>
       </c>
       <c r="AE12" s="1">
-        <v>1.1013645000000001</v>
+        <v>1.5171988999999999</v>
       </c>
       <c r="AF12" s="1">
-        <v>7.3486859999999998</v>
+        <v>13.916565</v>
       </c>
       <c r="AG12" s="1">
-        <v>14.77</v>
+        <v>8.15</v>
       </c>
       <c r="AH12" s="1">
-        <v>1684108800</v>
+        <v>1715644800</v>
       </c>
       <c r="AI12" s="1">
-        <v>3.58</v>
+        <v>3.72</v>
       </c>
       <c r="AJ12" s="1">
-        <v>3.4299999999999997E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="AK12" s="1">
-        <v>1686268800</v>
+        <v>1717977600</v>
       </c>
       <c r="AL12" s="1">
-        <v>3.64</v>
+        <v>3.8</v>
       </c>
       <c r="AM12" s="1">
-        <v>3.2986271999999997E-2</v>
+        <v>3.2772443999999998E-2</v>
       </c>
       <c r="AN12" s="1">
-        <v>3.58</v>
+        <v>3.72</v>
       </c>
       <c r="AO12" s="1">
-        <v>1682685000</v>
+        <v>1714134600</v>
       </c>
       <c r="AP12" s="1">
-        <v>2.2086581999999999</v>
+        <v>2.1788911999999998</v>
       </c>
       <c r="AQ12" s="1">
-        <v>49.143000000000001</v>
+        <v>52.054000000000002</v>
       </c>
       <c r="AR12" s="1">
-        <v>9.27</v>
+        <v>9.7100000000000009</v>
       </c>
       <c r="AS12" s="1">
-        <v>-1.02</v>
+        <v>1.88</v>
       </c>
       <c r="AT12" s="1">
-        <v>11.708748</v>
+        <v>11.680740999999999</v>
       </c>
       <c r="AU12" s="1">
-        <v>94863998976</v>
+        <v>67689000960</v>
       </c>
       <c r="AV12" s="1">
-        <v>2.15</v>
+        <v>6.23</v>
       </c>
       <c r="AW12" s="1" t="str">
         <v>--</v>
@@ -3613,133 +3616,133 @@
         <v>USD</v>
       </c>
       <c r="AY12" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="AZ12" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="BA12" s="1">
-        <v>108.53</v>
+        <v>113.51</v>
       </c>
       <c r="BB12" s="1">
-        <v>9.3073975000000002E-5</v>
+        <v>-7.9291699999999997E-4</v>
       </c>
       <c r="BC12" s="1" t="str">
-        <v>108.1 - 109.14</v>
+        <v>113.035 - 115.08</v>
       </c>
       <c r="BD12" s="1">
-        <v>14641530</v>
+        <v>15135050</v>
       </c>
       <c r="BE12" s="1">
         <v>0</v>
       </c>
       <c r="BF12" s="1">
-        <v>110.2976</v>
+        <v>117.5722</v>
       </c>
       <c r="BG12" s="1">
-        <v>-1.7574997000000001</v>
+        <v>-4.1521990000000004</v>
       </c>
       <c r="BH12" s="1">
-        <v>-1.5934159999999999E-2</v>
+        <v>-3.5316159999999999E-2</v>
       </c>
       <c r="BI12" s="1">
-        <v>107.01560000000001</v>
+        <v>109.08975</v>
       </c>
       <c r="BJ12" s="1">
-        <v>1.5244979999999999</v>
+        <v>4.3302459999999998</v>
       </c>
       <c r="BK12" s="1">
-        <v>1.4245568E-2</v>
+        <v>3.9694343E-2</v>
       </c>
       <c r="BL12" s="1" t="str">
-        <v>80.69 - 119.92</v>
+        <v>95.77 - 123.75</v>
       </c>
       <c r="BM12" s="1">
-        <v>80.69</v>
+        <v>95.77</v>
       </c>
       <c r="BN12" s="1">
-        <v>27.850097999999999</v>
+        <v>17.650002000000001</v>
       </c>
       <c r="BO12" s="1">
-        <v>0.34514929999999999</v>
+        <v>0.18429572999999999</v>
       </c>
       <c r="BP12" s="1">
-        <v>119.92</v>
+        <v>123.75</v>
       </c>
       <c r="BQ12" s="1">
-        <v>-11.379898000000001</v>
+        <v>-10.330002</v>
       </c>
       <c r="BR12" s="1">
-        <v>-9.4895750000000001E-2</v>
-      </c>
-      <c r="BS12" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT12" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU12" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV12" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW12" s="1">
-        <v>1686230990</v>
-      </c>
-      <c r="BX12" s="1">
-        <v>108.95</v>
-      </c>
-      <c r="BY12" s="1">
-        <v>0.41999799999999998</v>
-      </c>
-      <c r="BZ12" s="1">
-        <v>3.86988E-3</v>
+        <v>-8.3474759999999995E-2</v>
+      </c>
+      <c r="BS12" s="1">
+        <v>1716595170</v>
+      </c>
+      <c r="BT12" s="1">
+        <v>113.5</v>
+      </c>
+      <c r="BU12" s="1">
+        <v>8.0001829999999996E-2</v>
+      </c>
+      <c r="BV12" s="1">
+        <v>7.0535909999999995E-4</v>
+      </c>
+      <c r="BW12" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX12" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY12" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ12" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA12" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB12" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC12" s="1">
-        <v>0.44052083333333336</v>
+        <v>0.66833333333333333</v>
       </c>
       <c r="CD12" s="1">
-        <v>45061</v>
+        <v>45426</v>
       </c>
       <c r="CE12" s="1">
-        <v>45086</v>
+        <v>45453</v>
       </c>
       <c r="CF12" s="1">
-        <v>45044</v>
-      </c>
-      <c r="CG12" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH12" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI12" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ12" s="1">
-        <v>0.39571759263333334</v>
+        <v>45408</v>
+      </c>
+      <c r="CG12" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH12" s="1">
+        <v>0.83298611113333332</v>
+      </c>
+      <c r="CI12" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ12" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK12" s="1">
-        <v>45085.440520833334</v>
-      </c>
-      <c r="CL12" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM12" s="1">
-        <v>45085.395717592633</v>
+        <v>45436.668333333335</v>
+      </c>
+      <c r="CL12" s="1">
+        <v>45436.832986111134</v>
+      </c>
+      <c r="CM12" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN12" s="1">
-        <v>45134</v>
+        <v>45499</v>
       </c>
       <c r="CO12" s="1">
-        <v>45138</v>
+        <v>45503</v>
       </c>
     </row>
     <row r="13" spans="2:101" x14ac:dyDescent="0.25">
@@ -3750,7 +3753,7 @@
         <v>XOM240621C00115000</v>
       </c>
       <c r="D13" s="19" t="str">
-        <v>--</v>
+        <v>XOM Jun 2024 115.000 call</v>
       </c>
       <c r="E13" s="17" t="str">
         <v>XOM Jun 2024 115.000 call</v>
@@ -3789,31 +3792,31 @@
         <v>Delayed Quote</v>
       </c>
       <c r="Q13" s="10">
-        <v>9.5299999999999994</v>
+        <v>1.63</v>
       </c>
       <c r="R13" s="1">
-        <v>1686231759</v>
+        <v>1716580786</v>
       </c>
       <c r="S13" s="13">
-        <v>-0.119999886</v>
+        <v>-0.15999996999999999</v>
       </c>
       <c r="T13" s="1">
-        <v>9.5299999999999994</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="U13" s="1">
-        <v>9.5299999999999994</v>
+        <v>2.56</v>
       </c>
       <c r="V13" s="1">
-        <v>9.5299999999999994</v>
+        <v>1.48</v>
       </c>
       <c r="W13" s="1">
-        <v>1</v>
+        <v>702</v>
       </c>
       <c r="X13" s="1">
-        <v>9.65</v>
+        <v>1.6</v>
       </c>
       <c r="Y13" s="1">
-        <v>9.8000000000000007</v>
+        <v>1.65</v>
       </c>
       <c r="Z13" s="1" t="str">
         <v>--</v>
@@ -3897,13 +3900,13 @@
         <v>--</v>
       </c>
       <c r="BA13" s="1">
-        <v>9.65</v>
+        <v>1.79</v>
       </c>
       <c r="BB13" s="1">
-        <v>-1.2435221999999999E-2</v>
+        <v>-8.9385450000000005E-2</v>
       </c>
       <c r="BC13" s="1" t="str">
-        <v>9.53 - 9.53</v>
+        <v>1.48 - 2.56</v>
       </c>
       <c r="BD13" s="1" t="str">
         <v>--</v>
@@ -3930,25 +3933,25 @@
         <v>--</v>
       </c>
       <c r="BL13" s="1" t="str">
-        <v>9.53 - 9.53</v>
+        <v>1.48 - 2.56</v>
       </c>
       <c r="BM13" s="1">
-        <v>9.5299999999999994</v>
+        <v>1.48</v>
       </c>
       <c r="BN13" s="1">
-        <v>0</v>
+        <v>0.14999998</v>
       </c>
       <c r="BO13" s="1">
-        <v>0</v>
+        <v>0.101351336</v>
       </c>
       <c r="BP13" s="1">
-        <v>9.5299999999999994</v>
+        <v>2.56</v>
       </c>
       <c r="BQ13" s="1">
-        <v>0</v>
+        <v>-0.92999995000000002</v>
       </c>
       <c r="BR13" s="1">
-        <v>0</v>
+        <v>-0.36328125</v>
       </c>
       <c r="BS13" s="1" t="str">
         <v>--</v>
@@ -3978,10 +3981,10 @@
         <v>false</v>
       </c>
       <c r="CB13" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC13" s="1">
-        <v>0.40461805553333335</v>
+        <v>0.66650462963333335</v>
       </c>
       <c r="CD13" s="1" t="str">
         <v>--</v>
@@ -4005,7 +4008,7 @@
         <v>--</v>
       </c>
       <c r="CK13" s="1">
-        <v>45085.404618055531</v>
+        <v>45436.666504629633</v>
       </c>
       <c r="CL13" s="1" t="str">
         <v>--</v>
@@ -4319,7 +4322,7 @@
         <v>us_market</v>
       </c>
       <c r="I15" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J15" s="11">
         <v>15</v>
@@ -4343,40 +4346,40 @@
         <v>Nasdaq Real Time Price</v>
       </c>
       <c r="Q15" s="10">
-        <v>427.32</v>
+        <v>529.44000000000005</v>
       </c>
       <c r="R15" s="1">
-        <v>1686234861</v>
+        <v>1716580800</v>
       </c>
       <c r="S15" s="13">
-        <v>0.77001953000000001</v>
+        <v>3.4799799999999999</v>
       </c>
       <c r="T15" s="1">
-        <v>426.62</v>
+        <v>527.85</v>
       </c>
       <c r="U15" s="1">
-        <v>427.63</v>
+        <v>530.27</v>
       </c>
       <c r="V15" s="1">
-        <v>425.82</v>
+        <v>526.88099999999997</v>
       </c>
       <c r="W15" s="1">
-        <v>12011522</v>
+        <v>41291076</v>
       </c>
       <c r="X15" s="1">
-        <v>427.13</v>
+        <v>529.38</v>
       </c>
       <c r="Y15" s="1">
-        <v>427.02</v>
+        <v>529.69000000000005</v>
       </c>
       <c r="Z15" s="1">
         <v>917782016</v>
       </c>
       <c r="AA15" s="1">
-        <v>392186626048</v>
+        <v>485910511616</v>
       </c>
       <c r="AB15" s="1">
-        <v>88198046</v>
+        <v>66793588</v>
       </c>
       <c r="AC15" s="1" t="str">
         <v>--</v>
@@ -4388,7 +4391,7 @@
         <v>--</v>
       </c>
       <c r="AF15" s="1">
-        <v>21.526022000000001</v>
+        <v>26.670262999999998</v>
       </c>
       <c r="AG15" s="1">
         <v>19.851322</v>
@@ -4400,7 +4403,7 @@
         <v>--</v>
       </c>
       <c r="AJ15" s="1">
-        <v>1.55E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="AK15" s="1" t="str">
         <v>--</v>
@@ -4409,7 +4412,7 @@
         <v>--</v>
       </c>
       <c r="AM15" s="1">
-        <v>1.3273943E-2</v>
+        <v>1.0765078000000001E-2</v>
       </c>
       <c r="AN15" s="1">
         <v>5.6619999999999999</v>
@@ -4418,7 +4421,7 @@
         <v>--</v>
       </c>
       <c r="AP15" s="1">
-        <v>0.99557340000000005</v>
+        <v>1.2334932999999999</v>
       </c>
       <c r="AQ15" s="1">
         <v>429.22</v>
@@ -4445,97 +4448,97 @@
         <v>USD</v>
       </c>
       <c r="AY15" s="1">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AZ15" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="BA15" s="1">
-        <v>426.55</v>
+        <v>525.96</v>
       </c>
       <c r="BB15" s="1">
-        <v>1.805227E-3</v>
+        <v>6.6164400000000003E-3</v>
       </c>
       <c r="BC15" s="1" t="str">
-        <v>425.82 - 427.63</v>
+        <v>526.881 - 530.27</v>
       </c>
       <c r="BD15" s="1">
-        <v>85193330</v>
+        <v>48125040</v>
       </c>
       <c r="BE15" s="1">
         <v>0</v>
       </c>
       <c r="BF15" s="1">
-        <v>413.08679999999998</v>
+        <v>515.70339999999999</v>
       </c>
       <c r="BG15" s="1">
-        <v>14.233215</v>
+        <v>13.736572000000001</v>
       </c>
       <c r="BH15" s="1">
-        <v>3.445575E-2</v>
+        <v>2.6636573E-2</v>
       </c>
       <c r="BI15" s="1">
-        <v>396.62204000000003</v>
+        <v>474.57693</v>
       </c>
       <c r="BJ15" s="1">
-        <v>30.697967999999999</v>
+        <v>54.863067999999998</v>
       </c>
       <c r="BK15" s="1">
-        <v>7.7398540000000002E-2</v>
+        <v>0.11560416</v>
       </c>
       <c r="BL15" s="1" t="str">
-        <v>348.11 - 431.73</v>
+        <v>409.21 - 533.07</v>
       </c>
       <c r="BM15" s="1">
-        <v>348.11</v>
+        <v>409.21</v>
       </c>
       <c r="BN15" s="1">
-        <v>79.21002</v>
+        <v>120.23000999999999</v>
       </c>
       <c r="BO15" s="1">
-        <v>0.22754309</v>
+        <v>0.29381006999999998</v>
       </c>
       <c r="BP15" s="1">
-        <v>431.73</v>
+        <v>533.07000000000005</v>
       </c>
       <c r="BQ15" s="1">
-        <v>-4.4100036999999999</v>
+        <v>-3.6300050000000001</v>
       </c>
       <c r="BR15" s="1">
-        <v>-1.0214725500000001E-2</v>
-      </c>
-      <c r="BS15" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT15" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU15" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV15" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW15" s="1">
-        <v>1686230999</v>
-      </c>
-      <c r="BX15" s="1">
-        <v>426.59</v>
-      </c>
-      <c r="BY15" s="1">
-        <v>4.0008500000000002E-2</v>
-      </c>
-      <c r="BZ15" s="1">
-        <v>9.3795700000000001E-5</v>
+        <v>-6.8096210000000001E-3</v>
+      </c>
+      <c r="BS15" s="1">
+        <v>1716595197</v>
+      </c>
+      <c r="BT15" s="1">
+        <v>529.39</v>
+      </c>
+      <c r="BU15" s="1">
+        <v>-5.0109899999999999E-2</v>
+      </c>
+      <c r="BV15" s="1">
+        <v>-9.4646899999999997E-5</v>
+      </c>
+      <c r="BW15" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX15" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY15" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ15" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA15" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB15" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC15" s="1">
-        <v>0.44052083333333336</v>
+        <v>0.66666666663333329</v>
       </c>
       <c r="CD15" s="1" t="str">
         <v>--</v>
@@ -4546,26 +4549,26 @@
       <c r="CF15" s="1" t="str">
         <v>--</v>
       </c>
-      <c r="CG15" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH15" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI15" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ15" s="1">
-        <v>0.39582175923333335</v>
+      <c r="CG15" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH15" s="1">
+        <v>0.83329861113333337</v>
+      </c>
+      <c r="CI15" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ15" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK15" s="1">
-        <v>45085.440520833334</v>
-      </c>
-      <c r="CL15" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM15" s="1">
-        <v>45085.39582175923</v>
+        <v>45436.666666666635</v>
+      </c>
+      <c r="CL15" s="1">
+        <v>45436.833298611127</v>
+      </c>
+      <c r="CM15" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN15" s="1" t="str">
         <v>--</v>
@@ -4597,7 +4600,7 @@
         <v>us_market</v>
       </c>
       <c r="I16" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J16" s="11">
         <v>15</v>
@@ -4621,40 +4624,40 @@
         <v>Nasdaq Real Time Price</v>
       </c>
       <c r="Q16" s="10">
-        <v>185.55</v>
+        <v>205.44</v>
       </c>
       <c r="R16" s="1">
-        <v>1686234860</v>
+        <v>1716580800</v>
       </c>
       <c r="S16" s="13">
-        <v>-1.6900024</v>
+        <v>2.25</v>
       </c>
       <c r="T16" s="1">
-        <v>186.75</v>
+        <v>204.79</v>
       </c>
       <c r="U16" s="1">
-        <v>187.37</v>
+        <v>205.68</v>
       </c>
       <c r="V16" s="1">
-        <v>184.98</v>
+        <v>203.96</v>
       </c>
       <c r="W16" s="1">
-        <v>10656163</v>
+        <v>19946111</v>
       </c>
       <c r="X16" s="1">
-        <v>185.53</v>
+        <v>205.3</v>
       </c>
       <c r="Y16" s="1">
-        <v>185.54</v>
+        <v>205.41</v>
       </c>
       <c r="Z16" s="1">
         <v>281049984</v>
       </c>
       <c r="AA16" s="1">
-        <v>52148826112</v>
+        <v>57738907648</v>
       </c>
       <c r="AB16" s="1">
-        <v>34720636</v>
+        <v>31234580</v>
       </c>
       <c r="AC16" s="1" t="str">
         <v>--</v>
@@ -4666,7 +4669,7 @@
         <v>--</v>
       </c>
       <c r="AF16" s="1">
-        <v>11.831175</v>
+        <v>13.099416</v>
       </c>
       <c r="AG16" s="1">
         <v>15.683142999999999</v>
@@ -4678,7 +4681,7 @@
         <v>--</v>
       </c>
       <c r="AJ16" s="1">
-        <v>1.6199999999999999E-2</v>
+        <v>1.3299999999999999E-2</v>
       </c>
       <c r="AK16" s="1" t="str">
         <v>--</v>
@@ -4687,7 +4690,7 @@
         <v>--</v>
       </c>
       <c r="AM16" s="1">
-        <v>1.077227E-2</v>
+        <v>9.9266690000000008E-3</v>
       </c>
       <c r="AN16" s="1">
         <v>2.0169999999999999</v>
@@ -4696,7 +4699,7 @@
         <v>--</v>
       </c>
       <c r="AP16" s="1">
-        <v>0.84844580000000003</v>
+        <v>0.93939479999999997</v>
       </c>
       <c r="AQ16" s="1">
         <v>218.69399999999999</v>
@@ -4723,97 +4726,97 @@
         <v>USD</v>
       </c>
       <c r="AY16" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AZ16" s="1">
         <v>8</v>
       </c>
       <c r="BA16" s="1">
-        <v>187.24</v>
+        <v>203.19</v>
       </c>
       <c r="BB16" s="1">
-        <v>-9.0258620000000008E-3</v>
+        <v>1.1073400000000001E-2</v>
       </c>
       <c r="BC16" s="1" t="str">
-        <v>184.98 - 187.37</v>
+        <v>203.96 - 205.68</v>
       </c>
       <c r="BD16" s="1">
-        <v>38663980</v>
+        <v>25107890</v>
       </c>
       <c r="BE16" s="1">
         <v>0</v>
       </c>
       <c r="BF16" s="1">
-        <v>175.9204</v>
+        <v>202.78020000000001</v>
       </c>
       <c r="BG16" s="1">
-        <v>9.6296079999999993</v>
+        <v>2.6598052999999999</v>
       </c>
       <c r="BH16" s="1">
-        <v>5.4738439999999999E-2</v>
+        <v>1.3116691E-2</v>
       </c>
       <c r="BI16" s="1">
-        <v>179.69114999999999</v>
+        <v>190.79239999999999</v>
       </c>
       <c r="BJ16" s="1">
-        <v>5.8588560000000003</v>
+        <v>14.647598</v>
       </c>
       <c r="BK16" s="1">
-        <v>3.2605145000000002E-2</v>
+        <v>7.6772439999999997E-2</v>
       </c>
       <c r="BL16" s="1" t="str">
-        <v>162.5 - 201.99</v>
+        <v>161.67 - 211.88</v>
       </c>
       <c r="BM16" s="1">
-        <v>162.5</v>
+        <v>161.66999999999999</v>
       </c>
       <c r="BN16" s="1">
-        <v>23.050003</v>
+        <v>43.770004</v>
       </c>
       <c r="BO16" s="1">
-        <v>0.14184617999999999</v>
+        <v>0.27073671999999999</v>
       </c>
       <c r="BP16" s="1">
-        <v>201.99</v>
+        <v>211.88</v>
       </c>
       <c r="BQ16" s="1">
-        <v>-16.440002</v>
+        <v>-6.4400024</v>
       </c>
       <c r="BR16" s="1">
-        <v>-8.1390180000000006E-2</v>
-      </c>
-      <c r="BS16" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BT16" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BU16" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BV16" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BW16" s="1">
-        <v>1686230999</v>
-      </c>
-      <c r="BX16" s="1">
-        <v>186.71</v>
-      </c>
-      <c r="BY16" s="1">
-        <v>-0.529999</v>
-      </c>
-      <c r="BZ16" s="1">
-        <v>-2.83059E-3</v>
+        <v>-3.0394575E-2</v>
+      </c>
+      <c r="BS16" s="1">
+        <v>1716595197</v>
+      </c>
+      <c r="BT16" s="1">
+        <v>205.41</v>
+      </c>
+      <c r="BU16" s="1">
+        <v>-2.9998799999999999E-2</v>
+      </c>
+      <c r="BV16" s="1">
+        <v>-1.4602199999999999E-4</v>
+      </c>
+      <c r="BW16" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BX16" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BY16" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="BZ16" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CA16" s="1" t="str">
         <v>false</v>
       </c>
       <c r="CB16" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC16" s="1">
-        <v>0.44050925923333334</v>
+        <v>0.66666666663333329</v>
       </c>
       <c r="CD16" s="1" t="str">
         <v>--</v>
@@ -4824,26 +4827,26 @@
       <c r="CF16" s="1" t="str">
         <v>--</v>
       </c>
-      <c r="CG16" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CH16" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CI16" s="1">
-        <v>45085</v>
-      </c>
-      <c r="CJ16" s="1">
-        <v>0.39582175923333335</v>
+      <c r="CG16" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CH16" s="1">
+        <v>0.83329861113333337</v>
+      </c>
+      <c r="CI16" s="1" t="str">
+        <v>--</v>
+      </c>
+      <c r="CJ16" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CK16" s="1">
-        <v>45085.440509259235</v>
-      </c>
-      <c r="CL16" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CM16" s="1">
-        <v>45085.39582175923</v>
+        <v>45436.666666666635</v>
+      </c>
+      <c r="CL16" s="1">
+        <v>45436.833298611127</v>
+      </c>
+      <c r="CM16" s="1" t="str">
+        <v>--</v>
       </c>
       <c r="CN16" s="1" t="str">
         <v>--</v>
@@ -5151,7 +5154,7 @@
         <v>us_market</v>
       </c>
       <c r="I18" s="10" t="str">
-        <v>REGULAR</v>
+        <v>CLOSED</v>
       </c>
       <c r="J18" s="11">
         <v>15</v>
@@ -5175,13 +5178,13 @@
         <v>Delayed Quote</v>
       </c>
       <c r="Q18" s="10">
-        <v>394.86</v>
+        <v>490.48</v>
       </c>
       <c r="R18" s="1">
-        <v>1686225986</v>
+        <v>1716595292</v>
       </c>
       <c r="S18" s="13">
-        <v>-1.5</v>
+        <v>3.42</v>
       </c>
       <c r="T18" s="1" t="str">
         <v>--</v>
@@ -5220,7 +5223,7 @@
         <v>--</v>
       </c>
       <c r="AF18" s="1">
-        <v>21.345413000000001</v>
+        <v>26.514458000000001</v>
       </c>
       <c r="AG18" s="1">
         <v>18.498587000000001</v>
@@ -5229,19 +5232,19 @@
         <v>--</v>
       </c>
       <c r="AI18" s="1">
-        <v>1.391</v>
+        <v>1.4187000000000001</v>
       </c>
       <c r="AJ18" s="1">
-        <v>1.47E-2</v>
+        <v>1.29E-2</v>
       </c>
       <c r="AK18" s="1" t="str">
         <v>--</v>
       </c>
       <c r="AL18" s="1">
-        <v>1.391</v>
+        <v>1.4187000000000001</v>
       </c>
       <c r="AM18" s="1">
-        <v>1.3717327E-2</v>
+        <v>1.1162896E-2</v>
       </c>
       <c r="AN18" s="1">
         <v>5.4370000000000003</v>
@@ -5250,7 +5253,7 @@
         <v>--</v>
       </c>
       <c r="AP18" s="1">
-        <v>1.0102492999999999</v>
+        <v>1.2548931999999999</v>
       </c>
       <c r="AQ18" s="1">
         <v>390.85399999999998</v>
@@ -5283,10 +5286,10 @@
         <v>--</v>
       </c>
       <c r="BA18" s="1">
-        <v>396.36</v>
+        <v>487.06</v>
       </c>
       <c r="BB18" s="1">
-        <v>-3.7844387E-3</v>
+        <v>7.0217220000000002E-3</v>
       </c>
       <c r="BC18" s="1" t="str">
         <v>--</v>
@@ -5298,43 +5301,43 @@
         <v>0</v>
       </c>
       <c r="BF18" s="1">
-        <v>382.44540000000001</v>
+        <v>477.80540000000002</v>
       </c>
       <c r="BG18" s="1">
-        <v>12.414581</v>
+        <v>12.674621999999999</v>
       </c>
       <c r="BH18" s="1">
-        <v>3.2461055000000003E-2</v>
+        <v>2.6526745000000001E-2</v>
       </c>
       <c r="BI18" s="1">
-        <v>367.34910000000002</v>
+        <v>439.59359999999998</v>
       </c>
       <c r="BJ18" s="1">
-        <v>27.510895000000001</v>
+        <v>50.886414000000002</v>
       </c>
       <c r="BK18" s="1">
-        <v>7.4890330000000005E-2</v>
+        <v>0.11575786</v>
       </c>
       <c r="BL18" s="1" t="str">
-        <v>330.25 - 398.07</v>
+        <v>380.19 - 491.99</v>
       </c>
       <c r="BM18" s="1">
-        <v>330.25</v>
+        <v>380.19</v>
       </c>
       <c r="BN18" s="1">
-        <v>64.609984999999995</v>
+        <v>110.29001</v>
       </c>
       <c r="BO18" s="1">
-        <v>0.19563963000000001</v>
+        <v>0.29009180000000001</v>
       </c>
       <c r="BP18" s="1">
-        <v>398.07</v>
+        <v>491.99</v>
       </c>
       <c r="BQ18" s="1">
-        <v>-3.2100219999999999</v>
+        <v>-1.5099792000000001</v>
       </c>
       <c r="BR18" s="1">
-        <v>-8.0639639999999999E-3</v>
+        <v>-3.0691260000000001E-3</v>
       </c>
       <c r="BS18" s="1" t="str">
         <v>--</v>
@@ -5364,10 +5367,10 @@
         <v>false</v>
       </c>
       <c r="CB18" s="1">
-        <v>45085</v>
+        <v>45436</v>
       </c>
       <c r="CC18" s="1">
-        <v>0.33780092593333333</v>
+        <v>0.83439814813333324</v>
       </c>
       <c r="CD18" s="1" t="str">
         <v>--</v>
@@ -5391,7 +5394,7 @@
         <v>--</v>
       </c>
       <c r="CK18" s="1">
-        <v>45085.337800925932</v>
+        <v>45436.834398148138</v>
       </c>
       <c r="CL18" s="1" t="str">
         <v>--</v>
@@ -5683,210 +5686,212 @@
       </c>
     </row>
     <row r="20" spans="2:93" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
+      <c r="B20" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="C20" s="4" t="str">
-        <v>--</v>
+        <v>RY.TO</v>
       </c>
       <c r="D20" s="19" t="str">
-        <v>--</v>
+        <v>Royal Bank of Canada</v>
       </c>
       <c r="E20" s="17" t="str">
-        <v>--</v>
+        <v>ROYAL BANK OF CANADA</v>
       </c>
       <c r="F20" s="21" t="str">
-        <v>--</v>
+        <v>TOR</v>
       </c>
       <c r="G20" s="17" t="str">
-        <v>--</v>
+        <v>Toronto</v>
       </c>
       <c r="H20" s="10" t="str">
-        <v>--</v>
+        <v>ca_market</v>
       </c>
       <c r="I20" s="10" t="str">
-        <v>--</v>
-      </c>
-      <c r="J20" s="11" t="str">
-        <v>--</v>
+        <v>REGULAR</v>
+      </c>
+      <c r="J20" s="11">
+        <v>15</v>
       </c>
       <c r="K20" s="10" t="str">
-        <v>--</v>
+        <v>America/Toronto</v>
       </c>
       <c r="L20" s="4" t="str">
-        <v>--</v>
-      </c>
-      <c r="M20" s="10" t="str">
-        <v>--</v>
+        <v>EDT</v>
+      </c>
+      <c r="M20" s="10">
+        <v>-14400000</v>
       </c>
       <c r="N20" s="4" t="str">
-        <v>--</v>
+        <v>en-US</v>
       </c>
       <c r="O20" s="10" t="str">
-        <v>--</v>
+        <v>EQUITY</v>
       </c>
       <c r="P20" s="12" t="str">
-        <v>--</v>
-      </c>
-      <c r="Q20" s="10" t="str">
-        <v>--</v>
-      </c>
-      <c r="R20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="S20" s="13" t="str">
-        <v>--</v>
-      </c>
-      <c r="T20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="U20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="V20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="W20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="X20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="Y20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="Z20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AA20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AB20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AC20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AD20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AE20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AF20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AG20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AH20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AI20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AJ20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AK20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AL20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AM20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AN20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AO20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AP20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AQ20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AR20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AS20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AT20" s="1" t="str">
-        <v>--</v>
+        <v>Free Realtime Quote</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>143.75</v>
+      </c>
+      <c r="R20" s="1">
+        <v>1716830722</v>
+      </c>
+      <c r="S20" s="13">
+        <v>-0.16999817</v>
+      </c>
+      <c r="T20" s="1">
+        <v>143.81</v>
+      </c>
+      <c r="U20" s="1">
+        <v>144.28</v>
+      </c>
+      <c r="V20" s="1">
+        <v>143.61000000000001</v>
+      </c>
+      <c r="W20" s="1">
+        <v>176264</v>
+      </c>
+      <c r="X20" s="1">
+        <v>143.71</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>143.74</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>1413890048</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>203246698496</v>
+      </c>
+      <c r="AB20" s="1">
+        <v>4582714</v>
+      </c>
+      <c r="AC20" s="1">
+        <v>146.07</v>
+      </c>
+      <c r="AD20" s="1">
+        <v>53508002000</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>3.7984357000000002</v>
+      </c>
+      <c r="AF20" s="1">
+        <v>13.34726</v>
+      </c>
+      <c r="AG20" s="1">
+        <v>10.77</v>
+      </c>
+      <c r="AH20" s="1">
+        <v>1713916800</v>
+      </c>
+      <c r="AI20" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="AJ20" s="1">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="AK20" s="1">
+        <v>1716508800</v>
+      </c>
+      <c r="AL20" s="1">
+        <v>5.52</v>
+      </c>
+      <c r="AM20" s="1">
+        <v>3.7520843999999998E-2</v>
+      </c>
+      <c r="AN20" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="AO20" s="1">
+        <v>1717072200</v>
+      </c>
+      <c r="AP20" s="1">
+        <v>1.8681932999999999</v>
+      </c>
+      <c r="AQ20" s="1">
+        <v>76.945999999999998</v>
+      </c>
+      <c r="AR20" s="1">
+        <v>12.17</v>
+      </c>
+      <c r="AS20" s="1">
+        <v>2.08</v>
+      </c>
+      <c r="AT20" s="1">
+        <v>11.811832000000001</v>
       </c>
       <c r="AU20" s="1" t="str">
         <v>--</v>
       </c>
-      <c r="AV20" s="1" t="str">
-        <v>--</v>
+      <c r="AV20" s="1">
+        <v>1.75</v>
       </c>
       <c r="AW20" s="1" t="str">
         <v>--</v>
       </c>
       <c r="AX20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AY20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="AZ20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BA20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BB20" s="1" t="str">
-        <v>--</v>
+        <v>CAD</v>
+      </c>
+      <c r="AY20" s="1">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="1">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="1">
+        <v>143.91999999999999</v>
+      </c>
+      <c r="BB20" s="1">
+        <v>-1.1811991E-3</v>
       </c>
       <c r="BC20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BD20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BE20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BF20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BG20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BH20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BI20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BJ20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BK20" s="1" t="str">
-        <v>--</v>
+        <v>143.61 - 144.28</v>
+      </c>
+      <c r="BD20" s="1">
+        <v>4459980</v>
+      </c>
+      <c r="BE20" s="1">
+        <v>15</v>
+      </c>
+      <c r="BF20" s="1">
+        <v>137.48920000000001</v>
+      </c>
+      <c r="BG20" s="1">
+        <v>6.2608030000000001</v>
+      </c>
+      <c r="BH20" s="1">
+        <v>4.5536693000000003E-2</v>
+      </c>
+      <c r="BI20" s="1">
+        <v>127.8741</v>
+      </c>
+      <c r="BJ20" s="1">
+        <v>15.8759</v>
+      </c>
+      <c r="BK20" s="1">
+        <v>0.124152586</v>
       </c>
       <c r="BL20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BM20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BN20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BO20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BP20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BQ20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="BR20" s="1" t="str">
-        <v>--</v>
+        <v>107.92 - 145.75</v>
+      </c>
+      <c r="BM20" s="1">
+        <v>107.92</v>
+      </c>
+      <c r="BN20" s="1">
+        <v>35.83</v>
+      </c>
+      <c r="BO20" s="1">
+        <v>0.3320052</v>
+      </c>
+      <c r="BP20" s="1">
+        <v>145.75</v>
+      </c>
+      <c r="BQ20" s="1">
+        <v>-2</v>
+      </c>
+      <c r="BR20" s="1">
+        <v>-1.3722127000000001E-2</v>
       </c>
       <c r="BS20" s="1" t="str">
         <v>--</v>
@@ -5913,22 +5918,22 @@
         <v>--</v>
       </c>
       <c r="CA20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CB20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CC20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CD20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CE20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CF20" s="1" t="str">
-        <v>--</v>
+        <v>false</v>
+      </c>
+      <c r="CB20" s="1">
+        <v>45439</v>
+      </c>
+      <c r="CC20" s="1">
+        <v>0.55928240743333335</v>
+      </c>
+      <c r="CD20" s="1">
+        <v>45406</v>
+      </c>
+      <c r="CE20" s="1">
+        <v>45436</v>
+      </c>
+      <c r="CF20" s="1">
+        <v>45442</v>
       </c>
       <c r="CG20" s="1" t="str">
         <v>--</v>
@@ -5942,8 +5947,8 @@
       <c r="CJ20" s="1" t="str">
         <v>--</v>
       </c>
-      <c r="CK20" s="1" t="str">
-        <v>--</v>
+      <c r="CK20" s="1">
+        <v>45439.559282407434</v>
       </c>
       <c r="CL20" s="1" t="str">
         <v>--</v>
@@ -5951,11 +5956,11 @@
       <c r="CM20" s="1" t="str">
         <v>--</v>
       </c>
-      <c r="CN20" s="1" t="str">
-        <v>--</v>
-      </c>
-      <c r="CO20" s="1" t="str">
-        <v>--</v>
+      <c r="CN20" s="1">
+        <v>45442</v>
+      </c>
+      <c r="CO20" s="1">
+        <v>45442</v>
       </c>
     </row>
     <row r="21" spans="2:93" x14ac:dyDescent="0.25">

</xml_diff>